<commit_message>
try and find solid ground
Former-commit-id: 46e2457a048b10fe658ff214d616eac0ad86508e
</commit_message>
<xml_diff>
--- a/docs/20171205_lib2_ind/20171205.growth.xlsx
+++ b/docs/20171205_lib2_ind/20171205.growth.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="460" windowWidth="25600" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
@@ -156,6 +156,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -426,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>

</xml_diff>